<commit_message>
minor updates to discussion sections on schedule
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taylorokonek/Desktop/git/BIOST311/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E82C82E4-2D33-A24E-99BA-BB5C763C648C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{476D14E1-163C-E340-A82D-3F16FDE3B781}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28040" windowHeight="16500" xr2:uid="{0395EB9D-C0FC-FA49-A97A-D3904F742CDB}"/>
+    <workbookView xWindow="-34380" yWindow="3920" windowWidth="28040" windowHeight="16500" xr2:uid="{0395EB9D-C0FC-FA49-A97A-D3904F742CDB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="70">
   <si>
     <t>Date</t>
   </si>
@@ -313,12 +313,6 @@
     <t>Graphs &amp; descriptive statistics</t>
   </si>
   <si>
-    <t>SAPs and rubric, statistical -&gt; scientific question</t>
-  </si>
-  <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>Work on SAP</t>
   </si>
   <si>
@@ -389,6 +383,15 @@
   </si>
   <si>
     <t>Project</t>
+  </si>
+  <si>
+    <t>Scientific -&gt; statistical question</t>
+  </si>
+  <si>
+    <t>More on linear regression in R</t>
+  </si>
+  <si>
+    <t>Scientific paper critique?</t>
   </si>
 </sst>
 </file>
@@ -554,30 +557,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -590,53 +569,77 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="16" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -954,572 +957,581 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C6DA234-FFB9-4A4E-A4C5-173C0F365ED7}">
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" style="31" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" style="22" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.83203125" style="6" customWidth="1"/>
     <col min="3" max="3" width="72.6640625" style="6" customWidth="1"/>
     <col min="4" max="4" width="6.33203125" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="28.5" style="6" customWidth="1"/>
-    <col min="6" max="6" width="15.33203125" style="36" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" style="27" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.33203125" style="6" customWidth="1"/>
     <col min="8" max="8" width="35" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="H1" s="33" t="s">
+      <c r="G1" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" s="24" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="25">
+      <c r="A2" s="16">
         <v>44648</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="28" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="F2" s="22"/>
+      <c r="F2" s="13"/>
       <c r="G2" s="5"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="25">
+      <c r="A3" s="16">
         <v>44650</v>
       </c>
-      <c r="B3" s="8"/>
+      <c r="B3" s="29"/>
       <c r="C3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="22"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="13"/>
       <c r="G3" s="5"/>
     </row>
     <row r="4" spans="1:8" ht="54" x14ac:dyDescent="0.3">
-      <c r="A4" s="25">
+      <c r="A4" s="16">
         <v>44652</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="34" t="s">
+      <c r="B4" s="29"/>
+      <c r="C4" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="22"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="13"/>
       <c r="G4" s="5"/>
     </row>
     <row r="5" spans="1:8" ht="54" x14ac:dyDescent="0.3">
-      <c r="A5" s="25">
+      <c r="A5" s="16">
         <v>44655</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="34" t="s">
+      <c r="B5" s="29"/>
+      <c r="C5" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="7" t="s">
+      <c r="D5" s="33"/>
+      <c r="E5" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="F5" s="22"/>
+      <c r="F5" s="13"/>
       <c r="G5" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="54" x14ac:dyDescent="0.3">
-      <c r="A6" s="25">
+      <c r="A6" s="16">
         <v>44657</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="34" t="s">
+      <c r="B6" s="29"/>
+      <c r="C6" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="11"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="22"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="13"/>
       <c r="G6" s="5"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="25">
+      <c r="A7" s="16">
         <v>44659</v>
       </c>
-      <c r="B7" s="8"/>
+      <c r="B7" s="29"/>
       <c r="C7" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="22" t="s">
-        <v>59</v>
+      <c r="D7" s="33"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="13" t="s">
+        <v>57</v>
       </c>
       <c r="G7" s="5"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="26">
+      <c r="A8" s="17">
         <v>44662</v>
       </c>
-      <c r="B8" s="9"/>
+      <c r="B8" s="30"/>
       <c r="C8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="21"/>
-      <c r="E8" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="F8" s="22"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="F8" s="13"/>
       <c r="G8" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:8" ht="54" x14ac:dyDescent="0.3">
-      <c r="A9" s="25">
+      <c r="A9" s="16">
         <v>44664</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="34" t="s">
+      <c r="C9" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="8"/>
-      <c r="F9" s="22"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="13"/>
       <c r="G9" s="5"/>
     </row>
     <row r="10" spans="1:8" ht="81" x14ac:dyDescent="0.3">
-      <c r="A10" s="25">
+      <c r="A10" s="16">
         <v>44666</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="34" t="s">
+      <c r="B10" s="35"/>
+      <c r="C10" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="16" t="s">
-        <v>65</v>
+      <c r="D10" s="33"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="8" t="s">
+        <v>63</v>
       </c>
       <c r="G10" s="5"/>
     </row>
     <row r="11" spans="1:8" ht="54" x14ac:dyDescent="0.3">
-      <c r="A11" s="25">
+      <c r="A11" s="16">
         <v>44669</v>
       </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="34" t="s">
+      <c r="B11" s="35"/>
+      <c r="C11" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="11"/>
-      <c r="E11" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="F11" s="22"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="F11" s="13"/>
       <c r="G11" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="25">
+      <c r="A12" s="16">
         <v>44671</v>
       </c>
-      <c r="B12" s="13"/>
+      <c r="B12" s="35"/>
       <c r="C12" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="22"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="13"/>
       <c r="G12" s="5"/>
     </row>
     <row r="13" spans="1:8" ht="27" x14ac:dyDescent="0.3">
-      <c r="A13" s="25">
+      <c r="A13" s="16">
         <v>44673</v>
       </c>
-      <c r="B13" s="13"/>
+      <c r="B13" s="35"/>
       <c r="C13" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="11"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="16" t="s">
-        <v>60</v>
+      <c r="D13" s="33"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="8" t="s">
+        <v>58</v>
       </c>
       <c r="G13" s="5"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="25">
+      <c r="A14" s="16">
         <v>44676</v>
       </c>
-      <c r="B14" s="13"/>
+      <c r="B14" s="35"/>
       <c r="C14" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="11"/>
-      <c r="E14" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="F14" s="22"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" s="13"/>
       <c r="G14" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="25">
+      <c r="A15" s="16">
         <v>44678</v>
       </c>
-      <c r="B15" s="13"/>
+      <c r="B15" s="35"/>
       <c r="C15" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="22"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="33"/>
+      <c r="F15" s="13"/>
       <c r="G15" s="5"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="25">
+      <c r="A16" s="16">
         <v>44680</v>
       </c>
-      <c r="B16" s="13"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="11"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="22" t="s">
-        <v>66</v>
+      <c r="D16" s="33"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="13" t="s">
+        <v>64</v>
       </c>
       <c r="G16" s="5"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="26">
+      <c r="A17" s="17">
         <v>44683</v>
       </c>
-      <c r="B17" s="14"/>
+      <c r="B17" s="36"/>
       <c r="C17" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D17" s="21"/>
-      <c r="E17" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="F17" s="22"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="F17" s="13"/>
       <c r="G17" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H17" s="3"/>
     </row>
     <row r="18" spans="1:8" ht="26" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="25">
+      <c r="A18" s="16">
         <v>44685</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="34" t="s">
         <v>31</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="D18" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="E18" s="8"/>
-      <c r="F18" s="22"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="13"/>
       <c r="G18" s="5"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="25">
+      <c r="A19" s="16">
         <v>44687</v>
       </c>
-      <c r="B19" s="13"/>
+      <c r="B19" s="35"/>
       <c r="C19" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D19" s="11"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="22" t="s">
-        <v>61</v>
+      <c r="D19" s="33"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="13" t="s">
+        <v>59</v>
       </c>
       <c r="G19" s="5"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="25">
+      <c r="A20" s="16">
         <v>44690</v>
       </c>
-      <c r="B20" s="13"/>
+      <c r="B20" s="35"/>
       <c r="C20" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D20" s="11"/>
-      <c r="E20" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="F20" s="22"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="F20" s="13"/>
       <c r="G20" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="27">
+      <c r="A21" s="18">
         <v>44692</v>
       </c>
-      <c r="B21" s="13"/>
+      <c r="B21" s="35"/>
       <c r="C21" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D21" s="11"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="22"/>
+      <c r="D21" s="33"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="13"/>
       <c r="G21" s="5"/>
-      <c r="H21" s="15"/>
+      <c r="H21" s="7"/>
     </row>
     <row r="22" spans="1:8" ht="26" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="25">
+      <c r="A22" s="16">
         <v>44694</v>
       </c>
-      <c r="B22" s="13"/>
+      <c r="B22" s="35"/>
       <c r="C22" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D22" s="11"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="22" t="s">
-        <v>62</v>
+      <c r="D22" s="33"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="13" t="s">
+        <v>60</v>
       </c>
       <c r="G22" s="5"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="27">
+      <c r="A23" s="18">
         <v>44697</v>
       </c>
-      <c r="B23" s="13"/>
+      <c r="B23" s="35"/>
       <c r="C23" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D23" s="11"/>
-      <c r="E23" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F23" s="22"/>
+      <c r="D23" s="33"/>
+      <c r="E23" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="F23" s="13"/>
       <c r="G23" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="H23" s="15"/>
+        <v>55</v>
+      </c>
+      <c r="H23" s="7"/>
     </row>
     <row r="24" spans="1:8" ht="26" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="28">
+      <c r="A24" s="19">
         <v>44699</v>
       </c>
-      <c r="B24" s="14"/>
+      <c r="B24" s="36"/>
       <c r="C24" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D24" s="21"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="22"/>
+      <c r="D24" s="32"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="13"/>
       <c r="G24" s="5"/>
       <c r="H24" s="3"/>
     </row>
     <row r="25" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="25">
+      <c r="A25" s="16">
         <v>44701</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B25" s="29" t="s">
         <v>11</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D25" s="10" t="s">
+      <c r="D25" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="E25" s="9"/>
-      <c r="F25" s="16" t="s">
-        <v>67</v>
+      <c r="E25" s="30"/>
+      <c r="F25" s="8" t="s">
+        <v>65</v>
       </c>
       <c r="G25" s="5"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="25">
+      <c r="A26" s="16">
         <v>44704</v>
       </c>
-      <c r="B26" s="8"/>
+      <c r="B26" s="29"/>
       <c r="C26" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D26" s="11"/>
-      <c r="E26" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="F26" s="22"/>
+      <c r="D26" s="33"/>
+      <c r="E26" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="F26" s="13"/>
       <c r="G26" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="25">
+      <c r="A27" s="16">
         <v>44706</v>
       </c>
-      <c r="B27" s="8"/>
+      <c r="B27" s="29"/>
       <c r="C27" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D27" s="11"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="22"/>
+      <c r="D27" s="33"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="13"/>
       <c r="G27" s="5"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" s="28">
+      <c r="A28" s="19">
         <v>44708</v>
       </c>
-      <c r="B28" s="9"/>
+      <c r="B28" s="30"/>
       <c r="C28" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D28" s="21"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="23"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="30"/>
+      <c r="F28" s="14"/>
       <c r="G28" s="4"/>
       <c r="H28" s="2"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="29">
+      <c r="A29" s="20">
         <v>44711</v>
       </c>
-      <c r="B29" s="17"/>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="35"/>
-      <c r="G29" s="18"/>
-      <c r="H29" s="19" t="s">
+      <c r="B29" s="9"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="11" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30" s="25">
+      <c r="A30" s="16">
         <v>44713</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="B30" s="29" t="s">
         <v>12</v>
       </c>
       <c r="C30" s="5"/>
-      <c r="D30" s="24" t="s">
+      <c r="D30" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="E30" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="F30" s="22" t="s">
-        <v>63</v>
+      <c r="E30" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="F30" s="13" t="s">
+        <v>61</v>
       </c>
       <c r="G30" s="5"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" s="28">
+      <c r="A31" s="19">
         <v>44715</v>
       </c>
-      <c r="B31" s="9"/>
+      <c r="B31" s="30"/>
       <c r="C31" s="4"/>
-      <c r="D31" s="23" t="s">
+      <c r="D31" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="E31" s="21"/>
-      <c r="F31" s="23"/>
+      <c r="E31" s="30"/>
+      <c r="F31" s="14"/>
       <c r="G31" s="4"/>
       <c r="H31" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" s="30" t="s">
+      <c r="A32" s="21" t="s">
         <v>8</v>
       </c>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
-      <c r="F32" s="22" t="s">
-        <v>68</v>
+      <c r="F32" s="13" t="s">
+        <v>66</v>
       </c>
       <c r="G32" s="5"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="30"/>
+      <c r="A33" s="21"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
-      <c r="F33" s="22"/>
+      <c r="F33" s="13"/>
       <c r="G33" s="5"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" s="30"/>
+      <c r="A34" s="21"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
-      <c r="F34" s="22"/>
+      <c r="F34" s="13"/>
       <c r="G34" s="5"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="30"/>
+      <c r="A35" s="21"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
-      <c r="F35" s="22"/>
+      <c r="F35" s="13"/>
       <c r="G35" s="5"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="30"/>
+      <c r="A36" s="21"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
       <c r="E36" s="5"/>
-      <c r="F36" s="22"/>
+      <c r="F36" s="13"/>
       <c r="G36" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="D2:D8"/>
+    <mergeCell ref="D9:D17"/>
+    <mergeCell ref="B25:B28"/>
+    <mergeCell ref="B18:B24"/>
+    <mergeCell ref="D18:D24"/>
+    <mergeCell ref="D25:D28"/>
+    <mergeCell ref="B2:B8"/>
+    <mergeCell ref="B9:B17"/>
     <mergeCell ref="E20:E22"/>
     <mergeCell ref="E23:E25"/>
     <mergeCell ref="E26:E28"/>
@@ -1530,15 +1542,6 @@
     <mergeCell ref="E11:E13"/>
     <mergeCell ref="E14:E16"/>
     <mergeCell ref="E17:E19"/>
-    <mergeCell ref="D2:D8"/>
-    <mergeCell ref="D9:D17"/>
-    <mergeCell ref="B25:B28"/>
-    <mergeCell ref="B18:B24"/>
-    <mergeCell ref="D18:D24"/>
-    <mergeCell ref="D25:D28"/>
-    <mergeCell ref="B2:B8"/>
-    <mergeCell ref="B9:B17"/>
-    <mergeCell ref="B30:B31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updates to syllabus and schedule
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taylorokonek/Desktop/git/BIOST311/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{476D14E1-163C-E340-A82D-3F16FDE3B781}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8E24C6C-C9B0-9D47-9292-AB57A1C5D03A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-34380" yWindow="3920" windowWidth="28040" windowHeight="16500" xr2:uid="{0395EB9D-C0FC-FA49-A97A-D3904F742CDB}"/>
+    <workbookView xWindow="160" yWindow="560" windowWidth="28040" windowHeight="16500" xr2:uid="{0395EB9D-C0FC-FA49-A97A-D3904F742CDB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="71">
   <si>
     <t>Date</t>
   </si>
@@ -307,9 +307,6 @@
     <t>Cox proportional hazards model</t>
   </si>
   <si>
-    <t>Intro to R and course project</t>
-  </si>
-  <si>
     <t>Graphs &amp; descriptive statistics</t>
   </si>
   <si>
@@ -392,6 +389,12 @@
   </si>
   <si>
     <t>Scientific paper critique?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intro to R </t>
+  </si>
+  <si>
+    <t>Make sure project guidelines are distributed</t>
   </si>
 </sst>
 </file>
@@ -614,9 +617,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -626,12 +626,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -639,6 +639,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -957,8 +960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C6DA234-FFB9-4A4E-A4C5-173C0F365ED7}">
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
@@ -993,7 +996,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H1" s="24" t="s">
         <v>6</v>
@@ -1003,17 +1006,17 @@
       <c r="A2" s="16">
         <v>44648</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="36" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="31" t="s">
+      <c r="D2" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="28" t="s">
-        <v>41</v>
+      <c r="E2" s="36" t="s">
+        <v>69</v>
       </c>
       <c r="F2" s="13"/>
       <c r="G2" s="5"/>
@@ -1022,12 +1025,12 @@
       <c r="A3" s="16">
         <v>44650</v>
       </c>
-      <c r="B3" s="29"/>
+      <c r="B3" s="28"/>
       <c r="C3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="33"/>
-      <c r="E3" s="29"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="28"/>
       <c r="F3" s="13"/>
       <c r="G3" s="5"/>
     </row>
@@ -1035,45 +1038,48 @@
       <c r="A4" s="16">
         <v>44652</v>
       </c>
-      <c r="B4" s="29"/>
+      <c r="B4" s="28"/>
       <c r="C4" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="33"/>
-      <c r="E4" s="30"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="29"/>
       <c r="F4" s="13"/>
       <c r="G4" s="5"/>
+      <c r="H4" s="1" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="5" spans="1:8" ht="54" x14ac:dyDescent="0.3">
       <c r="A5" s="16">
         <v>44655</v>
       </c>
-      <c r="B5" s="29"/>
+      <c r="B5" s="28"/>
       <c r="C5" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="33"/>
-      <c r="E5" s="28" t="s">
-        <v>42</v>
+      <c r="D5" s="31"/>
+      <c r="E5" s="36" t="s">
+        <v>41</v>
       </c>
       <c r="F5" s="13"/>
       <c r="G5" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="54" x14ac:dyDescent="0.3">
       <c r="A6" s="16">
         <v>44657</v>
       </c>
-      <c r="B6" s="29"/>
+      <c r="B6" s="28"/>
       <c r="C6" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="33"/>
-      <c r="E6" s="29"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="28"/>
       <c r="F6" s="13"/>
       <c r="G6" s="5"/>
     </row>
@@ -1081,14 +1087,14 @@
       <c r="A7" s="16">
         <v>44659</v>
       </c>
-      <c r="B7" s="29"/>
+      <c r="B7" s="28"/>
       <c r="C7" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="33"/>
-      <c r="E7" s="30"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="29"/>
       <c r="F7" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G7" s="5"/>
     </row>
@@ -1096,17 +1102,17 @@
       <c r="A8" s="17">
         <v>44662</v>
       </c>
-      <c r="B8" s="30"/>
+      <c r="B8" s="29"/>
       <c r="C8" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D8" s="32"/>
-      <c r="E8" s="28" t="s">
-        <v>67</v>
+      <c r="E8" s="36" t="s">
+        <v>66</v>
       </c>
       <c r="F8" s="13"/>
       <c r="G8" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H8" s="3"/>
     </row>
@@ -1114,16 +1120,16 @@
       <c r="A9" s="16">
         <v>44664</v>
       </c>
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="33" t="s">
         <v>30</v>
       </c>
       <c r="C9" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="31" t="s">
+      <c r="D9" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="29"/>
+      <c r="E9" s="28"/>
       <c r="F9" s="13"/>
       <c r="G9" s="5"/>
     </row>
@@ -1131,14 +1137,14 @@
       <c r="A10" s="16">
         <v>44666</v>
       </c>
-      <c r="B10" s="35"/>
+      <c r="B10" s="34"/>
       <c r="C10" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="33"/>
-      <c r="E10" s="30"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="29"/>
       <c r="F10" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G10" s="5"/>
     </row>
@@ -1146,29 +1152,29 @@
       <c r="A11" s="16">
         <v>44669</v>
       </c>
-      <c r="B11" s="35"/>
+      <c r="B11" s="34"/>
       <c r="C11" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="33"/>
-      <c r="E11" s="28" t="s">
-        <v>68</v>
+      <c r="D11" s="31"/>
+      <c r="E11" s="36" t="s">
+        <v>67</v>
       </c>
       <c r="F11" s="13"/>
       <c r="G11" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="16">
         <v>44671</v>
       </c>
-      <c r="B12" s="35"/>
+      <c r="B12" s="34"/>
       <c r="C12" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="33"/>
-      <c r="E12" s="29"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="28"/>
       <c r="F12" s="13"/>
       <c r="G12" s="5"/>
     </row>
@@ -1176,14 +1182,14 @@
       <c r="A13" s="16">
         <v>44673</v>
       </c>
-      <c r="B13" s="35"/>
+      <c r="B13" s="34"/>
       <c r="C13" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="33"/>
-      <c r="E13" s="30"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="29"/>
       <c r="F13" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G13" s="5"/>
     </row>
@@ -1191,29 +1197,29 @@
       <c r="A14" s="16">
         <v>44676</v>
       </c>
-      <c r="B14" s="35"/>
+      <c r="B14" s="34"/>
       <c r="C14" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="33"/>
-      <c r="E14" s="31" t="s">
-        <v>43</v>
+      <c r="D14" s="31"/>
+      <c r="E14" s="30" t="s">
+        <v>42</v>
       </c>
       <c r="F14" s="13"/>
       <c r="G14" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="16">
         <v>44678</v>
       </c>
-      <c r="B15" s="35"/>
+      <c r="B15" s="34"/>
       <c r="C15" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="33"/>
-      <c r="E15" s="33"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="31"/>
       <c r="F15" s="13"/>
       <c r="G15" s="5"/>
     </row>
@@ -1221,14 +1227,14 @@
       <c r="A16" s="16">
         <v>44680</v>
       </c>
-      <c r="B16" s="35"/>
+      <c r="B16" s="34"/>
       <c r="C16" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="33"/>
+      <c r="D16" s="31"/>
       <c r="E16" s="32"/>
       <c r="F16" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G16" s="5"/>
     </row>
@@ -1236,17 +1242,17 @@
       <c r="A17" s="17">
         <v>44683</v>
       </c>
-      <c r="B17" s="36"/>
+      <c r="B17" s="35"/>
       <c r="C17" s="4" t="s">
         <v>29</v>
       </c>
       <c r="D17" s="32"/>
-      <c r="E17" s="28" t="s">
-        <v>44</v>
+      <c r="E17" s="36" t="s">
+        <v>43</v>
       </c>
       <c r="F17" s="13"/>
       <c r="G17" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H17" s="3"/>
     </row>
@@ -1254,16 +1260,16 @@
       <c r="A18" s="16">
         <v>44685</v>
       </c>
-      <c r="B18" s="34" t="s">
+      <c r="B18" s="33" t="s">
         <v>31</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="31" t="s">
+      <c r="D18" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="E18" s="29"/>
+      <c r="E18" s="28"/>
       <c r="F18" s="13"/>
       <c r="G18" s="5"/>
     </row>
@@ -1271,14 +1277,14 @@
       <c r="A19" s="16">
         <v>44687</v>
       </c>
-      <c r="B19" s="35"/>
+      <c r="B19" s="34"/>
       <c r="C19" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D19" s="33"/>
-      <c r="E19" s="30"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="29"/>
       <c r="F19" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G19" s="5"/>
     </row>
@@ -1286,29 +1292,29 @@
       <c r="A20" s="16">
         <v>44690</v>
       </c>
-      <c r="B20" s="35"/>
+      <c r="B20" s="34"/>
       <c r="C20" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D20" s="33"/>
-      <c r="E20" s="28" t="s">
-        <v>45</v>
+      <c r="D20" s="31"/>
+      <c r="E20" s="36" t="s">
+        <v>44</v>
       </c>
       <c r="F20" s="13"/>
       <c r="G20" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="18">
         <v>44692</v>
       </c>
-      <c r="B21" s="35"/>
+      <c r="B21" s="34"/>
       <c r="C21" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D21" s="33"/>
-      <c r="E21" s="29"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="28"/>
       <c r="F21" s="13"/>
       <c r="G21" s="5"/>
       <c r="H21" s="7"/>
@@ -1317,14 +1323,14 @@
       <c r="A22" s="16">
         <v>44694</v>
       </c>
-      <c r="B22" s="35"/>
+      <c r="B22" s="34"/>
       <c r="C22" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D22" s="33"/>
-      <c r="E22" s="30"/>
+      <c r="D22" s="31"/>
+      <c r="E22" s="29"/>
       <c r="F22" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G22" s="5"/>
     </row>
@@ -1332,17 +1338,17 @@
       <c r="A23" s="18">
         <v>44697</v>
       </c>
-      <c r="B23" s="35"/>
+      <c r="B23" s="34"/>
       <c r="C23" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D23" s="33"/>
-      <c r="E23" s="28" t="s">
-        <v>46</v>
+      <c r="D23" s="31"/>
+      <c r="E23" s="36" t="s">
+        <v>45</v>
       </c>
       <c r="F23" s="13"/>
       <c r="G23" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H23" s="7"/>
     </row>
@@ -1350,12 +1356,12 @@
       <c r="A24" s="19">
         <v>44699</v>
       </c>
-      <c r="B24" s="36"/>
+      <c r="B24" s="35"/>
       <c r="C24" s="4" t="s">
         <v>36</v>
       </c>
       <c r="D24" s="32"/>
-      <c r="E24" s="29"/>
+      <c r="E24" s="28"/>
       <c r="F24" s="13"/>
       <c r="G24" s="5"/>
       <c r="H24" s="3"/>
@@ -1364,18 +1370,18 @@
       <c r="A25" s="16">
         <v>44701</v>
       </c>
-      <c r="B25" s="29" t="s">
+      <c r="B25" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D25" s="31" t="s">
+      <c r="D25" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="E25" s="30"/>
+      <c r="E25" s="29"/>
       <c r="F25" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G25" s="5"/>
     </row>
@@ -1383,29 +1389,29 @@
       <c r="A26" s="16">
         <v>44704</v>
       </c>
-      <c r="B26" s="29"/>
+      <c r="B26" s="28"/>
       <c r="C26" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D26" s="33"/>
-      <c r="E26" s="28" t="s">
-        <v>47</v>
+      <c r="D26" s="31"/>
+      <c r="E26" s="36" t="s">
+        <v>46</v>
       </c>
       <c r="F26" s="13"/>
       <c r="G26" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="16">
         <v>44706</v>
       </c>
-      <c r="B27" s="29"/>
+      <c r="B27" s="28"/>
       <c r="C27" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D27" s="33"/>
-      <c r="E27" s="29"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="28"/>
       <c r="F27" s="13"/>
       <c r="G27" s="5"/>
     </row>
@@ -1413,12 +1419,12 @@
       <c r="A28" s="19">
         <v>44708</v>
       </c>
-      <c r="B28" s="30"/>
+      <c r="B28" s="29"/>
       <c r="C28" s="4" t="s">
         <v>40</v>
       </c>
       <c r="D28" s="32"/>
-      <c r="E28" s="30"/>
+      <c r="E28" s="29"/>
       <c r="F28" s="14"/>
       <c r="G28" s="4"/>
       <c r="H28" s="2"/>
@@ -1441,18 +1447,18 @@
       <c r="A30" s="16">
         <v>44713</v>
       </c>
-      <c r="B30" s="29" t="s">
+      <c r="B30" s="28" t="s">
         <v>12</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="E30" s="28" t="s">
-        <v>69</v>
+      <c r="E30" s="36" t="s">
+        <v>68</v>
       </c>
       <c r="F30" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G30" s="5"/>
     </row>
@@ -1460,12 +1466,12 @@
       <c r="A31" s="19">
         <v>44715</v>
       </c>
-      <c r="B31" s="30"/>
+      <c r="B31" s="29"/>
       <c r="C31" s="4"/>
       <c r="D31" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="E31" s="30"/>
+      <c r="E31" s="29"/>
       <c r="F31" s="14"/>
       <c r="G31" s="4"/>
       <c r="H31" s="2" t="s">
@@ -1481,7 +1487,7 @@
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
       <c r="F32" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G32" s="5"/>
     </row>
@@ -1523,15 +1529,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="D2:D8"/>
-    <mergeCell ref="D9:D17"/>
-    <mergeCell ref="B25:B28"/>
-    <mergeCell ref="B18:B24"/>
-    <mergeCell ref="D18:D24"/>
-    <mergeCell ref="D25:D28"/>
-    <mergeCell ref="B2:B8"/>
-    <mergeCell ref="B9:B17"/>
     <mergeCell ref="E20:E22"/>
     <mergeCell ref="E23:E25"/>
     <mergeCell ref="E26:E28"/>
@@ -1542,6 +1539,15 @@
     <mergeCell ref="E11:E13"/>
     <mergeCell ref="E14:E16"/>
     <mergeCell ref="E17:E19"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="D2:D8"/>
+    <mergeCell ref="D9:D17"/>
+    <mergeCell ref="B25:B28"/>
+    <mergeCell ref="B18:B24"/>
+    <mergeCell ref="D18:D24"/>
+    <mergeCell ref="D25:D28"/>
+    <mergeCell ref="B2:B8"/>
+    <mergeCell ref="B9:B17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update schedule with quizzes
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taylorokonek/Desktop/git/BIOST311/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8D57C33-2AED-6347-A947-E985C27BE131}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95BE0982-7D3A-6F4B-A84F-E960BA0EB476}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="160" yWindow="560" windowWidth="28040" windowHeight="16500" xr2:uid="{0395EB9D-C0FC-FA49-A97A-D3904F742CDB}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="74">
   <si>
     <t>Date</t>
   </si>
@@ -398,6 +398,12 @@
   </si>
   <si>
     <t>Project (Due June 8th)</t>
+  </si>
+  <si>
+    <t>Quiz 9</t>
+  </si>
+  <si>
+    <t>Quiz 10</t>
   </si>
 </sst>
 </file>
@@ -966,8 +972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C6DA234-FFB9-4A4E-A4C5-173C0F365ED7}">
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
@@ -1038,7 +1044,9 @@
       <c r="D3" s="32"/>
       <c r="E3" s="29"/>
       <c r="F3" s="13"/>
-      <c r="G3" s="5"/>
+      <c r="G3" s="5" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="4" spans="1:8" ht="54" x14ac:dyDescent="0.3">
       <c r="A4" s="16">
@@ -1070,7 +1078,7 @@
       </c>
       <c r="F5" s="13"/>
       <c r="G5" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>61</v>
@@ -1118,7 +1126,7 @@
       </c>
       <c r="F8" s="13"/>
       <c r="G8" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H8" s="3"/>
     </row>
@@ -1168,7 +1176,7 @@
       </c>
       <c r="F11" s="13"/>
       <c r="G11" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
@@ -1213,7 +1221,7 @@
       </c>
       <c r="F14" s="13"/>
       <c r="G14" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
@@ -1258,7 +1266,7 @@
       </c>
       <c r="F17" s="13"/>
       <c r="G17" s="5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H17" s="3"/>
     </row>
@@ -1308,7 +1316,7 @@
       </c>
       <c r="F20" s="13"/>
       <c r="G20" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
@@ -1354,7 +1362,7 @@
       </c>
       <c r="F23" s="13"/>
       <c r="G23" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H23" s="7"/>
     </row>
@@ -1405,7 +1413,7 @@
       </c>
       <c r="F26" s="13"/>
       <c r="G26" s="5" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
@@ -1468,7 +1476,9 @@
       <c r="F30" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="G30" s="5"/>
+      <c r="G30" s="5" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="19">

</xml_diff>

<commit_message>
add week into schedule
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taylorokonek/Desktop/git/BIOST311/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95BE0982-7D3A-6F4B-A84F-E960BA0EB476}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A832319D-81FF-DB49-9161-18BEBF3D201B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="160" yWindow="560" windowWidth="28040" windowHeight="16500" xr2:uid="{0395EB9D-C0FC-FA49-A97A-D3904F742CDB}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="75">
   <si>
     <t>Date</t>
   </si>
@@ -405,6 +405,9 @@
   <si>
     <t>Quiz 10</t>
   </si>
+  <si>
+    <t>Week</t>
+  </si>
 </sst>
 </file>
 
@@ -448,7 +451,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -557,11 +560,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -629,6 +643,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -653,8 +670,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -970,602 +992,666 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C6DA234-FFB9-4A4E-A4C5-173C0F365ED7}">
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" style="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.83203125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="72.6640625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="6.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.5" style="6" customWidth="1"/>
-    <col min="6" max="6" width="17.83203125" style="27" customWidth="1"/>
-    <col min="7" max="7" width="15.33203125" style="6" customWidth="1"/>
-    <col min="8" max="8" width="35" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="39"/>
+    <col min="2" max="2" width="18.33203125" style="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.83203125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="72.6640625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="6.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.5" style="6" customWidth="1"/>
+    <col min="7" max="7" width="17.83203125" style="27" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" style="6" customWidth="1"/>
+    <col min="9" max="9" width="35" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="38" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="C1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="D1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="E1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="F1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="G1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="H1" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="I1" s="24" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="16">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="40">
+        <v>1</v>
+      </c>
+      <c r="B2" s="16">
         <v>44648</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="C2" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="31" t="s">
+      <c r="E2" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="37" t="s">
+      <c r="F2" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="F2" s="13"/>
-      <c r="G2" s="5"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="16">
+      <c r="G2" s="13"/>
+      <c r="H2" s="5"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="41"/>
+      <c r="B3" s="16">
         <v>44650</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="30"/>
+      <c r="D3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="32"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="5" t="s">
+      <c r="E3" s="33"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="54" x14ac:dyDescent="0.3">
-      <c r="A4" s="16">
+    <row r="4" spans="1:9" ht="54" x14ac:dyDescent="0.3">
+      <c r="A4" s="41"/>
+      <c r="B4" s="16">
         <v>44652</v>
       </c>
-      <c r="B4" s="29"/>
-      <c r="C4" s="25" t="s">
+      <c r="C4" s="30"/>
+      <c r="D4" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="32"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="1" t="s">
+      <c r="E4" s="33"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="54" x14ac:dyDescent="0.3">
-      <c r="A5" s="16">
+    <row r="5" spans="1:9" ht="54" x14ac:dyDescent="0.3">
+      <c r="A5" s="41">
+        <v>2</v>
+      </c>
+      <c r="B5" s="16">
         <v>44655</v>
       </c>
-      <c r="B5" s="29"/>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="30"/>
+      <c r="D5" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="32"/>
-      <c r="E5" s="37" t="s">
+      <c r="E5" s="33"/>
+      <c r="F5" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="F5" s="13"/>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="13"/>
+      <c r="H5" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="54" x14ac:dyDescent="0.3">
-      <c r="A6" s="16">
+    <row r="6" spans="1:9" ht="54" x14ac:dyDescent="0.3">
+      <c r="A6" s="41"/>
+      <c r="B6" s="16">
         <v>44657</v>
       </c>
-      <c r="B6" s="29"/>
-      <c r="C6" s="25" t="s">
+      <c r="C6" s="30"/>
+      <c r="D6" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="32"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="5"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="16">
+      <c r="E6" s="33"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="5"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="41"/>
+      <c r="B7" s="16">
         <v>44659</v>
       </c>
-      <c r="B7" s="29"/>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="30"/>
+      <c r="D7" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="32"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="13" t="s">
+      <c r="E7" s="33"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="G7" s="5"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="17">
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="41">
+        <v>3</v>
+      </c>
+      <c r="B8" s="17">
         <v>44662</v>
       </c>
-      <c r="B8" s="30"/>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="31"/>
+      <c r="D8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="33"/>
-      <c r="E8" s="37" t="s">
+      <c r="E8" s="34"/>
+      <c r="F8" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="F8" s="13"/>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="13"/>
+      <c r="H8" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="H8" s="3"/>
-    </row>
-    <row r="9" spans="1:8" ht="54" x14ac:dyDescent="0.3">
-      <c r="A9" s="16">
+      <c r="I8" s="3"/>
+    </row>
+    <row r="9" spans="1:9" ht="54" x14ac:dyDescent="0.3">
+      <c r="A9" s="41"/>
+      <c r="B9" s="16">
         <v>44664</v>
       </c>
-      <c r="B9" s="34" t="s">
+      <c r="C9" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="25" t="s">
+      <c r="D9" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="31" t="s">
+      <c r="E9" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="29"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="5"/>
-    </row>
-    <row r="10" spans="1:8" ht="81" x14ac:dyDescent="0.3">
-      <c r="A10" s="16">
+      <c r="F9" s="30"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="5"/>
+    </row>
+    <row r="10" spans="1:9" ht="81" x14ac:dyDescent="0.3">
+      <c r="A10" s="41"/>
+      <c r="B10" s="16">
         <v>44666</v>
       </c>
-      <c r="B10" s="35"/>
-      <c r="C10" s="25" t="s">
+      <c r="C10" s="36"/>
+      <c r="D10" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="32"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="8" t="s">
+      <c r="E10" s="33"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="G10" s="5"/>
-    </row>
-    <row r="11" spans="1:8" ht="54" x14ac:dyDescent="0.3">
-      <c r="A11" s="16">
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" spans="1:9" ht="54" x14ac:dyDescent="0.3">
+      <c r="A11" s="41">
+        <v>4</v>
+      </c>
+      <c r="B11" s="16">
         <v>44669</v>
       </c>
-      <c r="B11" s="35"/>
-      <c r="C11" s="25" t="s">
+      <c r="C11" s="36"/>
+      <c r="D11" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="32"/>
-      <c r="E11" s="37" t="s">
+      <c r="E11" s="33"/>
+      <c r="F11" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="F11" s="13"/>
-      <c r="G11" s="5" t="s">
+      <c r="G11" s="13"/>
+      <c r="H11" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="16">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="41"/>
+      <c r="B12" s="16">
         <v>44671</v>
       </c>
-      <c r="B12" s="35"/>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="36"/>
+      <c r="D12" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="32"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="5"/>
-    </row>
-    <row r="13" spans="1:8" ht="27" x14ac:dyDescent="0.3">
-      <c r="A13" s="16">
+      <c r="E12" s="33"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="5"/>
+    </row>
+    <row r="13" spans="1:9" ht="27" x14ac:dyDescent="0.3">
+      <c r="A13" s="41"/>
+      <c r="B13" s="16">
         <v>44673</v>
       </c>
-      <c r="B13" s="35"/>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="36"/>
+      <c r="D13" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="32"/>
-      <c r="E13" s="30"/>
-      <c r="F13" s="8" t="s">
+      <c r="E13" s="33"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="G13" s="5"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="16">
+      <c r="H13" s="5"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="41">
+        <v>5</v>
+      </c>
+      <c r="B14" s="16">
         <v>44676</v>
       </c>
-      <c r="B14" s="35"/>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="36"/>
+      <c r="D14" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="32"/>
-      <c r="E14" s="31" t="s">
+      <c r="E14" s="33"/>
+      <c r="F14" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="F14" s="13"/>
-      <c r="G14" s="5" t="s">
+      <c r="G14" s="13"/>
+      <c r="H14" s="5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="16">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="41"/>
+      <c r="B15" s="16">
         <v>44678</v>
       </c>
-      <c r="B15" s="35"/>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="36"/>
+      <c r="D15" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="32"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="5"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="16">
+      <c r="E15" s="33"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="5"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="41"/>
+      <c r="B16" s="16">
         <v>44680</v>
       </c>
-      <c r="B16" s="35"/>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="36"/>
+      <c r="D16" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="32"/>
       <c r="E16" s="33"/>
-      <c r="F16" s="13" t="s">
+      <c r="F16" s="34"/>
+      <c r="G16" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="G16" s="5"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="17">
+      <c r="H16" s="5"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="41">
+        <v>6</v>
+      </c>
+      <c r="B17" s="17">
         <v>44683</v>
       </c>
-      <c r="B17" s="36"/>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="37"/>
+      <c r="D17" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D17" s="33"/>
-      <c r="E17" s="37" t="s">
+      <c r="E17" s="34"/>
+      <c r="F17" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="F17" s="13"/>
-      <c r="G17" s="5" t="s">
+      <c r="G17" s="13"/>
+      <c r="H17" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="H17" s="3"/>
-    </row>
-    <row r="18" spans="1:8" ht="26" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="16">
+      <c r="I17" s="3"/>
+    </row>
+    <row r="18" spans="1:9" ht="26" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="41"/>
+      <c r="B18" s="16">
         <v>44685</v>
       </c>
-      <c r="B18" s="34" t="s">
+      <c r="C18" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="D18" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="31" t="s">
+      <c r="E18" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="E18" s="29"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="5"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="16">
+      <c r="F18" s="30"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="5"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="41"/>
+      <c r="B19" s="16">
         <v>44687</v>
       </c>
-      <c r="B19" s="35"/>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="36"/>
+      <c r="D19" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D19" s="32"/>
-      <c r="E19" s="30"/>
-      <c r="F19" s="13" t="s">
+      <c r="E19" s="33"/>
+      <c r="F19" s="31"/>
+      <c r="G19" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="G19" s="5"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="16">
+      <c r="H19" s="5"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="41">
+        <v>7</v>
+      </c>
+      <c r="B20" s="16">
         <v>44690</v>
       </c>
-      <c r="B20" s="35"/>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="36"/>
+      <c r="D20" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D20" s="32"/>
-      <c r="E20" s="37" t="s">
+      <c r="E20" s="33"/>
+      <c r="F20" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="F20" s="13"/>
-      <c r="G20" s="5" t="s">
+      <c r="G20" s="13"/>
+      <c r="H20" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="18">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="41"/>
+      <c r="B21" s="18">
         <v>44692</v>
       </c>
-      <c r="B21" s="35"/>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="36"/>
+      <c r="D21" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D21" s="32"/>
-      <c r="E21" s="29"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="7"/>
-    </row>
-    <row r="22" spans="1:8" ht="26" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="16">
+      <c r="E21" s="33"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="7"/>
+    </row>
+    <row r="22" spans="1:9" ht="26" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="41"/>
+      <c r="B22" s="16">
         <v>44694</v>
       </c>
-      <c r="B22" s="35"/>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="36"/>
+      <c r="D22" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D22" s="32"/>
-      <c r="E22" s="30"/>
-      <c r="F22" s="13" t="s">
+      <c r="E22" s="33"/>
+      <c r="F22" s="31"/>
+      <c r="G22" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="G22" s="5"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="18">
+      <c r="H22" s="5"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="41">
+        <v>8</v>
+      </c>
+      <c r="B23" s="18">
         <v>44697</v>
       </c>
-      <c r="B23" s="35"/>
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="36"/>
+      <c r="D23" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D23" s="32"/>
-      <c r="E23" s="37" t="s">
+      <c r="E23" s="33"/>
+      <c r="F23" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="F23" s="13"/>
-      <c r="G23" s="5" t="s">
+      <c r="G23" s="13"/>
+      <c r="H23" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="H23" s="7"/>
-    </row>
-    <row r="24" spans="1:8" ht="26" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="19">
+      <c r="I23" s="7"/>
+    </row>
+    <row r="24" spans="1:9" ht="26" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="41"/>
+      <c r="B24" s="19">
         <v>44699</v>
       </c>
-      <c r="B24" s="36"/>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="37"/>
+      <c r="D24" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D24" s="33"/>
-      <c r="E24" s="29"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="3"/>
-    </row>
-    <row r="25" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="16">
+      <c r="E24" s="34"/>
+      <c r="F24" s="30"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="3"/>
+    </row>
+    <row r="25" spans="1:9" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="41"/>
+      <c r="B25" s="16">
         <v>44701</v>
       </c>
-      <c r="B25" s="29" t="s">
+      <c r="C25" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="D25" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D25" s="31" t="s">
+      <c r="E25" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="E25" s="30"/>
-      <c r="F25" s="8" t="s">
+      <c r="F25" s="31"/>
+      <c r="G25" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="G25" s="5"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="16">
+      <c r="H25" s="5"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="41">
+        <v>9</v>
+      </c>
+      <c r="B26" s="16">
         <v>44704</v>
       </c>
-      <c r="B26" s="29"/>
-      <c r="C26" s="5" t="s">
+      <c r="C26" s="30"/>
+      <c r="D26" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D26" s="32"/>
-      <c r="E26" s="37" t="s">
+      <c r="E26" s="33"/>
+      <c r="F26" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="F26" s="13"/>
-      <c r="G26" s="5" t="s">
+      <c r="G26" s="13"/>
+      <c r="H26" s="5" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="16">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" s="41"/>
+      <c r="B27" s="16">
         <v>44706</v>
       </c>
-      <c r="B27" s="29"/>
-      <c r="C27" s="5" t="s">
+      <c r="C27" s="30"/>
+      <c r="D27" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D27" s="32"/>
-      <c r="E27" s="29"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="5"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" s="19">
+      <c r="E27" s="33"/>
+      <c r="F27" s="30"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="5"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" s="41"/>
+      <c r="B28" s="19">
         <v>44708</v>
       </c>
-      <c r="B28" s="30"/>
-      <c r="C28" s="4" t="s">
+      <c r="C28" s="31"/>
+      <c r="D28" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D28" s="33"/>
-      <c r="E28" s="30"/>
-      <c r="F28" s="14" t="s">
+      <c r="E28" s="34"/>
+      <c r="F28" s="31"/>
+      <c r="G28" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="G28" s="4"/>
-      <c r="H28" s="2"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="20">
+      <c r="H28" s="4"/>
+      <c r="I28" s="2"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" s="41">
+        <v>10</v>
+      </c>
+      <c r="B29" s="20">
         <v>44711</v>
       </c>
-      <c r="B29" s="9"/>
-      <c r="C29" s="10"/>
+      <c r="C29" s="9"/>
       <c r="D29" s="10"/>
       <c r="E29" s="10"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="11" t="s">
+      <c r="F29" s="10"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="10"/>
+      <c r="I29" s="11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30" s="16">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30" s="41"/>
+      <c r="B30" s="16">
         <v>44713</v>
       </c>
-      <c r="B30" s="29" t="s">
+      <c r="C30" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="C30" s="5"/>
-      <c r="D30" s="15" t="s">
+      <c r="D30" s="5"/>
+      <c r="E30" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="E30" s="37" t="s">
+      <c r="F30" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="F30" s="13" t="s">
+      <c r="G30" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="G30" s="5" t="s">
+      <c r="H30" s="5" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" s="19">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" s="41"/>
+      <c r="B31" s="19">
         <v>44715</v>
       </c>
-      <c r="B31" s="30"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="14" t="s">
+      <c r="C31" s="31"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="E31" s="30"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="2" t="s">
+      <c r="F31" s="31"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="81" x14ac:dyDescent="0.3">
-      <c r="A32" s="21" t="s">
+    <row r="32" spans="1:9" ht="81" x14ac:dyDescent="0.3">
+      <c r="B32" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
-      <c r="F32" s="28" t="s">
+      <c r="F32" s="5"/>
+      <c r="G32" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="G32" s="5"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="21"/>
-      <c r="B33" s="5"/>
+      <c r="H32" s="5"/>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B33" s="21"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="5"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" s="21"/>
-      <c r="B34" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="5"/>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B34" s="21"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="5"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="21"/>
-      <c r="B35" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="5"/>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B35" s="21"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="5"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="21"/>
-      <c r="B36" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="5"/>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B36" s="21"/>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
       <c r="E36" s="5"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="5"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="E20:E22"/>
-    <mergeCell ref="E23:E25"/>
-    <mergeCell ref="E26:E28"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="E2:E4"/>
-    <mergeCell ref="E5:E7"/>
-    <mergeCell ref="E8:E10"/>
-    <mergeCell ref="E11:E13"/>
-    <mergeCell ref="E14:E16"/>
-    <mergeCell ref="E17:E19"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="D2:D8"/>
-    <mergeCell ref="D9:D17"/>
-    <mergeCell ref="B25:B28"/>
-    <mergeCell ref="B18:B24"/>
-    <mergeCell ref="D18:D24"/>
-    <mergeCell ref="D25:D28"/>
-    <mergeCell ref="B2:B8"/>
-    <mergeCell ref="B9:B17"/>
+  <mergeCells count="29">
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="E2:E8"/>
+    <mergeCell ref="E9:E17"/>
+    <mergeCell ref="C25:C28"/>
+    <mergeCell ref="C18:C24"/>
+    <mergeCell ref="E18:E24"/>
+    <mergeCell ref="E25:E28"/>
+    <mergeCell ref="C2:C8"/>
+    <mergeCell ref="C9:C17"/>
+    <mergeCell ref="F20:F22"/>
+    <mergeCell ref="F23:F25"/>
+    <mergeCell ref="F26:F28"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="F2:F4"/>
+    <mergeCell ref="F5:F7"/>
+    <mergeCell ref="F8:F10"/>
+    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="F14:F16"/>
+    <mergeCell ref="F17:F19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update quiz section on syllabus
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taylorokonek/Desktop/git/BIOST311/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A832319D-81FF-DB49-9161-18BEBF3D201B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE8909A-2C5A-5449-83F9-7553C3361A55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="560" windowWidth="28040" windowHeight="16500" xr2:uid="{0395EB9D-C0FC-FA49-A97A-D3904F742CDB}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28040" windowHeight="16500" xr2:uid="{0395EB9D-C0FC-FA49-A97A-D3904F742CDB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="74">
   <si>
     <t>Date</t>
   </si>
@@ -367,9 +367,6 @@
     <t>HW8</t>
   </si>
   <si>
-    <t>Project groups assigned</t>
-  </si>
-  <si>
     <t>HW2, Project proposal</t>
   </si>
   <si>
@@ -643,40 +640,40 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -994,13 +991,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C6DA234-FFB9-4A4E-A4C5-173C0F365ED7}">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="39"/>
+    <col min="1" max="1" width="10.83203125" style="30"/>
     <col min="2" max="2" width="18.33203125" style="22" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.83203125" style="6" customWidth="1"/>
     <col min="4" max="4" width="72.6640625" style="6" customWidth="1"/>
@@ -1012,8 +1009,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="38" t="s">
-        <v>74</v>
+      <c r="A1" s="29" t="s">
+        <v>73</v>
       </c>
       <c r="B1" s="23" t="s">
         <v>0</v>
@@ -1041,127 +1038,124 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="40">
+      <c r="A2" s="32">
         <v>1</v>
       </c>
       <c r="B2" s="16">
         <v>44648</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="41" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="32" t="s">
+      <c r="E2" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="29" t="s">
-        <v>68</v>
+      <c r="F2" s="41" t="s">
+        <v>67</v>
       </c>
       <c r="G2" s="13"/>
       <c r="H2" s="5"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="41"/>
+      <c r="A3" s="31"/>
       <c r="B3" s="16">
         <v>44650</v>
       </c>
-      <c r="C3" s="30"/>
+      <c r="C3" s="33"/>
       <c r="D3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="33"/>
-      <c r="F3" s="30"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="33"/>
       <c r="G3" s="13"/>
       <c r="H3" s="5" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="54" x14ac:dyDescent="0.3">
-      <c r="A4" s="41"/>
+      <c r="A4" s="31"/>
       <c r="B4" s="16">
         <v>44652</v>
       </c>
-      <c r="C4" s="30"/>
+      <c r="C4" s="33"/>
       <c r="D4" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="33"/>
-      <c r="F4" s="31"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="34"/>
       <c r="G4" s="13"/>
       <c r="H4" s="5"/>
       <c r="I4" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="54" x14ac:dyDescent="0.3">
-      <c r="A5" s="41">
+      <c r="A5" s="31">
         <v>2</v>
       </c>
       <c r="B5" s="16">
         <v>44655</v>
       </c>
-      <c r="C5" s="30"/>
+      <c r="C5" s="33"/>
       <c r="D5" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="33"/>
-      <c r="F5" s="29" t="s">
+      <c r="E5" s="36"/>
+      <c r="F5" s="41" t="s">
         <v>41</v>
       </c>
       <c r="G5" s="13"/>
       <c r="H5" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="I5" s="1" t="s">
-        <v>61</v>
-      </c>
     </row>
     <row r="6" spans="1:9" ht="54" x14ac:dyDescent="0.3">
-      <c r="A6" s="41"/>
+      <c r="A6" s="31"/>
       <c r="B6" s="16">
         <v>44657</v>
       </c>
-      <c r="C6" s="30"/>
+      <c r="C6" s="33"/>
       <c r="D6" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="33"/>
-      <c r="F6" s="30"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="33"/>
       <c r="G6" s="13"/>
       <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="41"/>
+      <c r="A7" s="31"/>
       <c r="B7" s="16">
         <v>44659</v>
       </c>
-      <c r="C7" s="30"/>
+      <c r="C7" s="33"/>
       <c r="D7" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="33"/>
-      <c r="F7" s="31"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="34"/>
       <c r="G7" s="13" t="s">
         <v>56</v>
       </c>
       <c r="H7" s="5"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="41">
+      <c r="A8" s="31">
         <v>3</v>
       </c>
       <c r="B8" s="17">
         <v>44662</v>
       </c>
-      <c r="C8" s="31"/>
+      <c r="C8" s="34"/>
       <c r="D8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="34"/>
-      <c r="F8" s="29" t="s">
-        <v>65</v>
+      <c r="E8" s="37"/>
+      <c r="F8" s="41" t="s">
+        <v>64</v>
       </c>
       <c r="G8" s="13"/>
       <c r="H8" s="5" t="s">
@@ -1170,53 +1164,53 @@
       <c r="I8" s="3"/>
     </row>
     <row r="9" spans="1:9" ht="54" x14ac:dyDescent="0.3">
-      <c r="A9" s="41"/>
+      <c r="A9" s="31"/>
       <c r="B9" s="16">
         <v>44664</v>
       </c>
-      <c r="C9" s="35" t="s">
+      <c r="C9" s="38" t="s">
         <v>30</v>
       </c>
       <c r="D9" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="32" t="s">
+      <c r="E9" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="30"/>
+      <c r="F9" s="33"/>
       <c r="G9" s="13"/>
       <c r="H9" s="5"/>
     </row>
     <row r="10" spans="1:9" ht="81" x14ac:dyDescent="0.3">
-      <c r="A10" s="41"/>
+      <c r="A10" s="31"/>
       <c r="B10" s="16">
         <v>44666</v>
       </c>
-      <c r="C10" s="36"/>
+      <c r="C10" s="39"/>
       <c r="D10" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="33"/>
-      <c r="F10" s="31"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="34"/>
       <c r="G10" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H10" s="5"/>
     </row>
     <row r="11" spans="1:9" ht="54" x14ac:dyDescent="0.3">
-      <c r="A11" s="41">
+      <c r="A11" s="31">
         <v>4</v>
       </c>
       <c r="B11" s="16">
         <v>44669</v>
       </c>
-      <c r="C11" s="36"/>
+      <c r="C11" s="39"/>
       <c r="D11" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="33"/>
-      <c r="F11" s="29" t="s">
-        <v>66</v>
+      <c r="E11" s="36"/>
+      <c r="F11" s="41" t="s">
+        <v>65</v>
       </c>
       <c r="G11" s="13"/>
       <c r="H11" s="5" t="s">
@@ -1224,48 +1218,48 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="41"/>
+      <c r="A12" s="31"/>
       <c r="B12" s="16">
         <v>44671</v>
       </c>
-      <c r="C12" s="36"/>
+      <c r="C12" s="39"/>
       <c r="D12" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E12" s="33"/>
-      <c r="F12" s="30"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="33"/>
       <c r="G12" s="13"/>
       <c r="H12" s="5"/>
     </row>
     <row r="13" spans="1:9" ht="27" x14ac:dyDescent="0.3">
-      <c r="A13" s="41"/>
+      <c r="A13" s="31"/>
       <c r="B13" s="16">
         <v>44673</v>
       </c>
-      <c r="C13" s="36"/>
+      <c r="C13" s="39"/>
       <c r="D13" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E13" s="33"/>
-      <c r="F13" s="31"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="34"/>
       <c r="G13" s="8" t="s">
         <v>57</v>
       </c>
       <c r="H13" s="5"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="41">
+      <c r="A14" s="31">
         <v>5</v>
       </c>
       <c r="B14" s="16">
         <v>44676</v>
       </c>
-      <c r="C14" s="36"/>
+      <c r="C14" s="39"/>
       <c r="D14" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="33"/>
-      <c r="F14" s="32" t="s">
+      <c r="E14" s="36"/>
+      <c r="F14" s="35" t="s">
         <v>42</v>
       </c>
       <c r="G14" s="13"/>
@@ -1274,48 +1268,48 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="41"/>
+      <c r="A15" s="31"/>
       <c r="B15" s="16">
         <v>44678</v>
       </c>
-      <c r="C15" s="36"/>
+      <c r="C15" s="39"/>
       <c r="D15" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="33"/>
-      <c r="F15" s="33"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="36"/>
       <c r="G15" s="13"/>
       <c r="H15" s="5"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="41"/>
+      <c r="A16" s="31"/>
       <c r="B16" s="16">
         <v>44680</v>
       </c>
-      <c r="C16" s="36"/>
+      <c r="C16" s="39"/>
       <c r="D16" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E16" s="33"/>
-      <c r="F16" s="34"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="37"/>
       <c r="G16" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H16" s="5"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="41">
+      <c r="A17" s="31">
         <v>6</v>
       </c>
       <c r="B17" s="17">
         <v>44683</v>
       </c>
-      <c r="C17" s="37"/>
+      <c r="C17" s="40"/>
       <c r="D17" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E17" s="34"/>
-      <c r="F17" s="29" t="s">
+      <c r="E17" s="37"/>
+      <c r="F17" s="41" t="s">
         <v>43</v>
       </c>
       <c r="G17" s="13"/>
@@ -1325,52 +1319,52 @@
       <c r="I17" s="3"/>
     </row>
     <row r="18" spans="1:9" ht="26" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="41"/>
+      <c r="A18" s="31"/>
       <c r="B18" s="16">
         <v>44685</v>
       </c>
-      <c r="C18" s="35" t="s">
+      <c r="C18" s="38" t="s">
         <v>31</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E18" s="32" t="s">
+      <c r="E18" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="F18" s="30"/>
+      <c r="F18" s="33"/>
       <c r="G18" s="13"/>
       <c r="H18" s="5"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="41"/>
+      <c r="A19" s="31"/>
       <c r="B19" s="16">
         <v>44687</v>
       </c>
-      <c r="C19" s="36"/>
+      <c r="C19" s="39"/>
       <c r="D19" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E19" s="33"/>
-      <c r="F19" s="31"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="34"/>
       <c r="G19" s="13" t="s">
         <v>58</v>
       </c>
       <c r="H19" s="5"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="41">
+      <c r="A20" s="31">
         <v>7</v>
       </c>
       <c r="B20" s="16">
         <v>44690</v>
       </c>
-      <c r="C20" s="36"/>
+      <c r="C20" s="39"/>
       <c r="D20" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E20" s="33"/>
-      <c r="F20" s="29" t="s">
+      <c r="E20" s="36"/>
+      <c r="F20" s="41" t="s">
         <v>44</v>
       </c>
       <c r="G20" s="13"/>
@@ -1379,49 +1373,49 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="41"/>
+      <c r="A21" s="31"/>
       <c r="B21" s="18">
         <v>44692</v>
       </c>
-      <c r="C21" s="36"/>
+      <c r="C21" s="39"/>
       <c r="D21" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E21" s="33"/>
-      <c r="F21" s="30"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="33"/>
       <c r="G21" s="13"/>
       <c r="H21" s="5"/>
       <c r="I21" s="7"/>
     </row>
     <row r="22" spans="1:9" ht="26" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="41"/>
+      <c r="A22" s="31"/>
       <c r="B22" s="16">
         <v>44694</v>
       </c>
-      <c r="C22" s="36"/>
+      <c r="C22" s="39"/>
       <c r="D22" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="E22" s="33"/>
-      <c r="F22" s="31"/>
+      <c r="E22" s="36"/>
+      <c r="F22" s="34"/>
       <c r="G22" s="13" t="s">
         <v>59</v>
       </c>
       <c r="H22" s="5"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="41">
+      <c r="A23" s="31">
         <v>8</v>
       </c>
       <c r="B23" s="18">
         <v>44697</v>
       </c>
-      <c r="C23" s="36"/>
+      <c r="C23" s="39"/>
       <c r="D23" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="E23" s="33"/>
-      <c r="F23" s="29" t="s">
+      <c r="E23" s="36"/>
+      <c r="F23" s="41" t="s">
         <v>45</v>
       </c>
       <c r="G23" s="13"/>
@@ -1431,93 +1425,93 @@
       <c r="I23" s="7"/>
     </row>
     <row r="24" spans="1:9" ht="26" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="41"/>
+      <c r="A24" s="31"/>
       <c r="B24" s="19">
         <v>44699</v>
       </c>
-      <c r="C24" s="37"/>
+      <c r="C24" s="40"/>
       <c r="D24" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E24" s="34"/>
-      <c r="F24" s="30"/>
+      <c r="E24" s="37"/>
+      <c r="F24" s="33"/>
       <c r="G24" s="13"/>
       <c r="H24" s="5"/>
       <c r="I24" s="3"/>
     </row>
     <row r="25" spans="1:9" ht="54" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="41"/>
+      <c r="A25" s="31"/>
       <c r="B25" s="16">
         <v>44701</v>
       </c>
-      <c r="C25" s="30" t="s">
+      <c r="C25" s="33" t="s">
         <v>11</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E25" s="32" t="s">
+      <c r="E25" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="F25" s="31"/>
+      <c r="F25" s="34"/>
       <c r="G25" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H25" s="5"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="41">
+      <c r="A26" s="31">
         <v>9</v>
       </c>
       <c r="B26" s="16">
         <v>44704</v>
       </c>
-      <c r="C26" s="30"/>
+      <c r="C26" s="33"/>
       <c r="D26" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E26" s="33"/>
-      <c r="F26" s="29" t="s">
+      <c r="E26" s="36"/>
+      <c r="F26" s="41" t="s">
         <v>46</v>
       </c>
       <c r="G26" s="13"/>
       <c r="H26" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="41"/>
+      <c r="A27" s="31"/>
       <c r="B27" s="16">
         <v>44706</v>
       </c>
-      <c r="C27" s="30"/>
+      <c r="C27" s="33"/>
       <c r="D27" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="E27" s="33"/>
-      <c r="F27" s="30"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="33"/>
       <c r="G27" s="13"/>
       <c r="H27" s="5"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="41"/>
+      <c r="A28" s="31"/>
       <c r="B28" s="19">
         <v>44708</v>
       </c>
-      <c r="C28" s="31"/>
+      <c r="C28" s="34"/>
       <c r="D28" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E28" s="34"/>
-      <c r="F28" s="31"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="34"/>
       <c r="G28" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H28" s="4"/>
       <c r="I28" s="2"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="41">
+      <c r="A29" s="31">
         <v>10</v>
       </c>
       <c r="B29" s="20">
@@ -1534,38 +1528,38 @@
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="41"/>
+      <c r="A30" s="31"/>
       <c r="B30" s="16">
         <v>44713</v>
       </c>
-      <c r="C30" s="30" t="s">
+      <c r="C30" s="33" t="s">
         <v>12</v>
       </c>
       <c r="D30" s="5"/>
       <c r="E30" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="F30" s="29" t="s">
-        <v>67</v>
+      <c r="F30" s="41" t="s">
+        <v>66</v>
       </c>
       <c r="G30" s="13" t="s">
         <v>60</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="41"/>
+      <c r="A31" s="31"/>
       <c r="B31" s="19">
         <v>44715</v>
       </c>
-      <c r="C31" s="31"/>
+      <c r="C31" s="34"/>
       <c r="D31" s="4"/>
       <c r="E31" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="F31" s="31"/>
+      <c r="F31" s="34"/>
       <c r="G31" s="14"/>
       <c r="H31" s="4"/>
       <c r="I31" s="2" t="s">
@@ -1581,7 +1575,7 @@
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
       <c r="G32" s="28" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H32" s="5"/>
     </row>
@@ -1623,25 +1617,6 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="E2:E8"/>
-    <mergeCell ref="E9:E17"/>
-    <mergeCell ref="C25:C28"/>
-    <mergeCell ref="C18:C24"/>
-    <mergeCell ref="E18:E24"/>
-    <mergeCell ref="E25:E28"/>
-    <mergeCell ref="C2:C8"/>
-    <mergeCell ref="C9:C17"/>
     <mergeCell ref="F20:F22"/>
     <mergeCell ref="F23:F25"/>
     <mergeCell ref="F26:F28"/>
@@ -1652,6 +1627,25 @@
     <mergeCell ref="F11:F13"/>
     <mergeCell ref="F14:F16"/>
     <mergeCell ref="F17:F19"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="E2:E8"/>
+    <mergeCell ref="E9:E17"/>
+    <mergeCell ref="C25:C28"/>
+    <mergeCell ref="C18:C24"/>
+    <mergeCell ref="E18:E24"/>
+    <mergeCell ref="E25:E28"/>
+    <mergeCell ref="C2:C8"/>
+    <mergeCell ref="C9:C17"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="A29:A31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
hw5 key, hw6, updates to schedule, week7 section and week7 section key
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taylorokonek/Desktop/git/BIOST311/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9E3B81F-B95F-D04D-8372-D360EC4D869C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27A41C1D-0F1F-4543-AB52-841354D88D57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28040" windowHeight="16440" xr2:uid="{0395EB9D-C0FC-FA49-A97A-D3904F742CDB}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="88">
   <si>
     <t>Date</t>
   </si>
@@ -307,9 +307,6 @@
     <t>Work on SAP</t>
   </si>
   <si>
-    <t>Linear regression review</t>
-  </si>
-  <si>
     <t>Logistic regression overview</t>
   </si>
   <si>
@@ -434,6 +431,21 @@
   </si>
   <si>
     <t>Prediction in linear regression (through end of measures of prediction accuracy)</t>
+  </si>
+  <si>
+    <t>Prediction in linear regression (bonus slides), Summarizing binary outcomes</t>
+  </si>
+  <si>
+    <t>Simple linear regression with binary outcomes</t>
+  </si>
+  <si>
+    <t>Quizzes moved to Tuesdays starting with Quiz 7, HW due dates moved to Midnight on Friday instead of 12:30pm Friday starting with HW6</t>
+  </si>
+  <si>
+    <t>Simple &amp; Multiple logistic regression</t>
+  </si>
+  <si>
+    <t>T until here?</t>
   </si>
 </sst>
 </file>
@@ -602,7 +614,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -709,6 +721,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1025,8 +1043,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C6DA234-FFB9-4A4E-A4C5-173C0F365ED7}">
   <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
@@ -1040,12 +1058,12 @@
     <col min="8" max="8" width="28.5" style="6" customWidth="1"/>
     <col min="9" max="9" width="17.83203125" style="27" customWidth="1"/>
     <col min="10" max="10" width="15.33203125" style="6" customWidth="1"/>
-    <col min="11" max="11" width="35" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="69.6640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="29" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B1" s="23" t="s">
         <v>0</v>
@@ -1054,16 +1072,16 @@
         <v>1</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F1" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="G1" s="12" t="s">
         <v>74</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>75</v>
       </c>
       <c r="H1" s="12" t="s">
         <v>2</v>
@@ -1072,7 +1090,7 @@
         <v>3</v>
       </c>
       <c r="J1" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K1" s="24" t="s">
         <v>4</v>
@@ -1101,7 +1119,7 @@
         <v>11</v>
       </c>
       <c r="H2" s="31" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I2" s="13"/>
       <c r="J2" s="5"/>
@@ -1123,7 +1141,7 @@
       <c r="H3" s="32"/>
       <c r="I3" s="13"/>
       <c r="J3" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="54" x14ac:dyDescent="0.3">
@@ -1144,7 +1162,7 @@
       <c r="I4" s="13"/>
       <c r="J4" s="5"/>
       <c r="K4" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="54" x14ac:dyDescent="0.3">
@@ -1168,7 +1186,7 @@
       </c>
       <c r="I5" s="13"/>
       <c r="J5" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="54" x14ac:dyDescent="0.3">
@@ -1205,7 +1223,7 @@
       <c r="G7" s="35"/>
       <c r="H7" s="33"/>
       <c r="I7" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J7" s="5"/>
     </row>
@@ -1221,16 +1239,16 @@
         <v>18</v>
       </c>
       <c r="E8" s="25" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F8" s="35"/>
       <c r="G8" s="36"/>
       <c r="H8" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I8" s="13"/>
       <c r="J8" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K8" s="3"/>
     </row>
@@ -1246,7 +1264,7 @@
         <v>19</v>
       </c>
       <c r="E9" s="43" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F9" s="36"/>
       <c r="G9" s="40" t="s">
@@ -1266,13 +1284,15 @@
         <v>20</v>
       </c>
       <c r="E10" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="F10" s="25"/>
+        <v>70</v>
+      </c>
+      <c r="F10" s="31" t="s">
+        <v>12</v>
+      </c>
       <c r="G10" s="35"/>
       <c r="H10" s="33"/>
       <c r="I10" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J10" s="5"/>
     </row>
@@ -1290,14 +1310,14 @@
       <c r="E11" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="25"/>
+      <c r="F11" s="32"/>
       <c r="G11" s="35"/>
       <c r="H11" s="31" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I11" s="13"/>
       <c r="J11" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -1310,9 +1330,9 @@
         <v>22</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="F12" s="5"/>
+        <v>69</v>
+      </c>
+      <c r="F12" s="32"/>
       <c r="G12" s="35"/>
       <c r="H12" s="32"/>
       <c r="I12" s="13"/>
@@ -1328,13 +1348,13 @@
         <v>22</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F13" s="5"/>
+        <v>80</v>
+      </c>
+      <c r="F13" s="32"/>
       <c r="G13" s="35"/>
       <c r="H13" s="33"/>
       <c r="I13" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J13" s="5"/>
     </row>
@@ -1350,16 +1370,16 @@
         <v>24</v>
       </c>
       <c r="E14" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="F14" s="5"/>
+        <v>79</v>
+      </c>
+      <c r="F14" s="32"/>
       <c r="G14" s="35"/>
       <c r="H14" s="34" t="s">
         <v>40</v>
       </c>
       <c r="I14" s="13"/>
       <c r="J14" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="54" x14ac:dyDescent="0.3">
@@ -1372,9 +1392,9 @@
         <v>25</v>
       </c>
       <c r="E15" s="25" t="s">
-        <v>82</v>
-      </c>
-      <c r="F15" s="5"/>
+        <v>81</v>
+      </c>
+      <c r="F15" s="32"/>
       <c r="G15" s="35"/>
       <c r="H15" s="35"/>
       <c r="I15" s="13"/>
@@ -1390,17 +1410,17 @@
         <v>26</v>
       </c>
       <c r="E16" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="F16" s="5"/>
+        <v>82</v>
+      </c>
+      <c r="F16" s="32"/>
       <c r="G16" s="35"/>
       <c r="H16" s="36"/>
       <c r="I16" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J16" s="5"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" ht="54" x14ac:dyDescent="0.3">
       <c r="A17" s="41">
         <v>6</v>
       </c>
@@ -1411,15 +1431,17 @@
       <c r="D17" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
+      <c r="E17" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="F17" s="32"/>
       <c r="G17" s="36"/>
       <c r="H17" s="31" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="I17" s="13"/>
       <c r="J17" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K17" s="3"/>
     </row>
@@ -1434,8 +1456,10 @@
       <c r="D18" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
+      <c r="E18" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F18" s="33"/>
       <c r="G18" s="34" t="s">
         <v>11</v>
       </c>
@@ -1452,16 +1476,18 @@
       <c r="D19" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="E19" s="5"/>
+      <c r="E19" s="5" t="s">
+        <v>86</v>
+      </c>
       <c r="F19" s="5"/>
       <c r="G19" s="35"/>
       <c r="H19" s="33"/>
       <c r="I19" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J19" s="5"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" ht="81" x14ac:dyDescent="0.3">
       <c r="A20" s="41">
         <v>7</v>
       </c>
@@ -1476,11 +1502,14 @@
       <c r="F20" s="5"/>
       <c r="G20" s="35"/>
       <c r="H20" s="31" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I20" s="13"/>
       <c r="J20" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
+      </c>
+      <c r="K20" s="45" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
@@ -1498,7 +1527,6 @@
       <c r="H21" s="32"/>
       <c r="I21" s="13"/>
       <c r="J21" s="5"/>
-      <c r="K21" s="7"/>
     </row>
     <row r="22" spans="1:11" ht="26" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="41"/>
@@ -1514,7 +1542,7 @@
       <c r="G22" s="35"/>
       <c r="H22" s="33"/>
       <c r="I22" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J22" s="5"/>
     </row>
@@ -1533,11 +1561,11 @@
       <c r="F23" s="5"/>
       <c r="G23" s="35"/>
       <c r="H23" s="31" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I23" s="13"/>
       <c r="J23" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K23" s="7"/>
     </row>
@@ -1551,7 +1579,9 @@
         <v>34</v>
       </c>
       <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
+      <c r="F24" s="4" t="s">
+        <v>87</v>
+      </c>
       <c r="G24" s="36"/>
       <c r="H24" s="32"/>
       <c r="I24" s="13"/>
@@ -1576,7 +1606,7 @@
       </c>
       <c r="H25" s="33"/>
       <c r="I25" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J25" s="5"/>
     </row>
@@ -1595,11 +1625,11 @@
       <c r="F26" s="5"/>
       <c r="G26" s="35"/>
       <c r="H26" s="31" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I26" s="13"/>
       <c r="J26" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
@@ -1632,7 +1662,7 @@
       <c r="G28" s="36"/>
       <c r="H28" s="33"/>
       <c r="I28" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J28" s="4"/>
       <c r="K28" s="2"/>
@@ -1671,13 +1701,13 @@
         <v>11</v>
       </c>
       <c r="H30" s="31" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I30" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
@@ -1710,7 +1740,7 @@
       <c r="G32" s="5"/>
       <c r="H32" s="5"/>
       <c r="I32" s="28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J32" s="5"/>
     </row>
@@ -1759,7 +1789,7 @@
       <c r="J36" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="30">
+  <mergeCells count="31">
     <mergeCell ref="A17:A19"/>
     <mergeCell ref="A20:A22"/>
     <mergeCell ref="A23:A25"/>
@@ -1780,6 +1810,7 @@
     <mergeCell ref="C2:C8"/>
     <mergeCell ref="C9:C17"/>
     <mergeCell ref="F2:F9"/>
+    <mergeCell ref="F10:F18"/>
     <mergeCell ref="H20:H22"/>
     <mergeCell ref="H23:H25"/>
     <mergeCell ref="H26:H28"/>

</xml_diff>

<commit_message>
final updates to actual schedule (vs. planned)
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taylorokonek/Desktop/git/BIOST311/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C98553C9-AE73-6E40-82B3-08C8EB83807E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA256CB3-5FD7-B446-BA70-D64612661450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28040" windowHeight="16440" xr2:uid="{0395EB9D-C0FC-FA49-A97A-D3904F742CDB}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="96">
   <si>
     <t>Date</t>
   </si>
@@ -125,9 +125,6 @@
       </rPr>
       <t>Survival Analysis</t>
     </r>
-  </si>
-  <si>
-    <t>Special Topics?</t>
   </si>
   <si>
     <t>T</t>
@@ -355,9 +352,6 @@
     <t>HW7, Draft 1</t>
   </si>
   <si>
-    <t>Scientific paper critique?</t>
-  </si>
-  <si>
     <t xml:space="preserve">Intro to R </t>
   </si>
   <si>
@@ -439,19 +433,43 @@
     <t>Simple &amp; Multiple logistic regression</t>
   </si>
   <si>
-    <t>T until here?</t>
-  </si>
-  <si>
     <t>Logistic regression prediction</t>
   </si>
   <si>
-    <t>Survival overview</t>
-  </si>
-  <si>
     <t>Logistic regression prediction &amp; adjustment variables</t>
   </si>
   <si>
     <t>Logistic regression: case-control studies</t>
+  </si>
+  <si>
+    <t>Beginning of Kaplan-Meier subsection</t>
+  </si>
+  <si>
+    <t>Kaplan-Meier, building the estimator via probability &amp; via re-distribution to the right</t>
+  </si>
+  <si>
+    <t>Kaplan-Meier in R</t>
+  </si>
+  <si>
+    <t>Log rank test &amp; Cox proportional Hazards model</t>
+  </si>
+  <si>
+    <t>Survival Overview</t>
+  </si>
+  <si>
+    <t>Special Topics</t>
+  </si>
+  <si>
+    <t>Cox proportional Hazards model</t>
+  </si>
+  <si>
+    <t>Scientific paper critique</t>
+  </si>
+  <si>
+    <t>Spatial statistics &amp; Under-5 Mortality Estimation</t>
+  </si>
+  <si>
+    <t>Nonparametric Statistics</t>
   </si>
 </sst>
 </file>
@@ -620,7 +638,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -690,37 +708,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -732,6 +723,39 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1049,8 +1073,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C6DA234-FFB9-4A4E-A4C5-173C0F365ED7}">
   <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
@@ -1069,7 +1093,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="29" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B1" s="23" t="s">
         <v>0</v>
@@ -1078,16 +1102,16 @@
         <v>1</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H1" s="12" t="s">
         <v>2</v>
@@ -1096,591 +1120,605 @@
         <v>3</v>
       </c>
       <c r="J1" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K1" s="24" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="40">
+      <c r="A2" s="43">
         <v>1</v>
       </c>
       <c r="B2" s="16">
         <v>44648</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="37" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="31" t="s">
-        <v>58</v>
+        <v>12</v>
+      </c>
+      <c r="F2" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="37" t="s">
+        <v>56</v>
       </c>
       <c r="I2" s="13"/>
       <c r="J2" s="5"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="41"/>
+      <c r="A3" s="47"/>
       <c r="B3" s="16">
         <v>44650</v>
       </c>
-      <c r="C3" s="32"/>
+      <c r="C3" s="38"/>
       <c r="D3" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="32"/>
+        <v>13</v>
+      </c>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="38"/>
       <c r="I3" s="13"/>
       <c r="J3" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="54" x14ac:dyDescent="0.3">
-      <c r="A4" s="41"/>
+      <c r="A4" s="47"/>
       <c r="B4" s="16">
         <v>44652</v>
       </c>
-      <c r="C4" s="32"/>
+      <c r="C4" s="38"/>
       <c r="D4" s="25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E4" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="33"/>
+        <v>14</v>
+      </c>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="39"/>
       <c r="I4" s="13"/>
       <c r="J4" s="5"/>
       <c r="K4" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="54" x14ac:dyDescent="0.3">
-      <c r="A5" s="41">
+      <c r="A5" s="47">
         <v>2</v>
       </c>
       <c r="B5" s="16">
         <v>44655</v>
       </c>
-      <c r="C5" s="32"/>
+      <c r="C5" s="38"/>
       <c r="D5" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E5" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="31" t="s">
-        <v>39</v>
+        <v>15</v>
+      </c>
+      <c r="F5" s="41"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="37" t="s">
+        <v>38</v>
       </c>
       <c r="I5" s="13"/>
       <c r="J5" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="54" x14ac:dyDescent="0.3">
-      <c r="A6" s="41"/>
+      <c r="A6" s="47"/>
       <c r="B6" s="16">
         <v>44657</v>
       </c>
-      <c r="C6" s="32"/>
+      <c r="C6" s="38"/>
       <c r="D6" s="25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E6" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="32"/>
+        <v>16</v>
+      </c>
+      <c r="F6" s="41"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="38"/>
       <c r="I6" s="13"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="41"/>
+      <c r="A7" s="47"/>
       <c r="B7" s="16">
         <v>44659</v>
       </c>
-      <c r="C7" s="32"/>
+      <c r="C7" s="38"/>
       <c r="D7" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="35"/>
-      <c r="G7" s="35"/>
-      <c r="H7" s="33"/>
+        <v>22</v>
+      </c>
+      <c r="F7" s="41"/>
+      <c r="G7" s="41"/>
+      <c r="H7" s="39"/>
       <c r="I7" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:11" ht="54" x14ac:dyDescent="0.3">
-      <c r="A8" s="41">
+      <c r="A8" s="47">
         <v>3</v>
       </c>
       <c r="B8" s="17">
         <v>44662</v>
       </c>
-      <c r="C8" s="33"/>
+      <c r="C8" s="39"/>
       <c r="D8" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E8" s="25" t="s">
-        <v>69</v>
-      </c>
-      <c r="F8" s="35"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="31" t="s">
-        <v>73</v>
+        <v>67</v>
+      </c>
+      <c r="F8" s="41"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="37" t="s">
+        <v>71</v>
       </c>
       <c r="I8" s="13"/>
       <c r="J8" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K8" s="3"/>
     </row>
     <row r="9" spans="1:11" ht="54" x14ac:dyDescent="0.3">
-      <c r="A9" s="41"/>
+      <c r="A9" s="47"/>
       <c r="B9" s="16">
         <v>44664</v>
       </c>
-      <c r="C9" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" s="42" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" s="43" t="s">
-        <v>70</v>
-      </c>
-      <c r="F9" s="36"/>
-      <c r="G9" s="40" t="s">
-        <v>12</v>
-      </c>
-      <c r="H9" s="32"/>
+      <c r="C9" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="F9" s="42"/>
+      <c r="G9" s="43" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="38"/>
       <c r="I9" s="13"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:11" ht="81" x14ac:dyDescent="0.3">
-      <c r="A10" s="41"/>
+      <c r="A10" s="47"/>
       <c r="B10" s="16">
         <v>44666</v>
       </c>
-      <c r="C10" s="38"/>
+      <c r="C10" s="45"/>
       <c r="D10" s="25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E10" s="25" t="s">
-        <v>68</v>
-      </c>
-      <c r="F10" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10" s="35"/>
-      <c r="H10" s="33"/>
+        <v>66</v>
+      </c>
+      <c r="F10" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="41"/>
+      <c r="H10" s="39"/>
       <c r="I10" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:11" ht="54" x14ac:dyDescent="0.3">
-      <c r="A11" s="41">
+      <c r="A11" s="47">
         <v>4</v>
       </c>
       <c r="B11" s="16">
         <v>44669</v>
       </c>
-      <c r="C11" s="38"/>
+      <c r="C11" s="45"/>
       <c r="D11" s="25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E11" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="F11" s="32"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="31" t="s">
-        <v>74</v>
+        <v>18</v>
+      </c>
+      <c r="F11" s="38"/>
+      <c r="G11" s="41"/>
+      <c r="H11" s="37" t="s">
+        <v>72</v>
       </c>
       <c r="I11" s="13"/>
       <c r="J11" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="41"/>
+      <c r="A12" s="47"/>
       <c r="B12" s="16">
         <v>44671</v>
       </c>
-      <c r="C12" s="38"/>
+      <c r="C12" s="45"/>
       <c r="D12" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="F12" s="32"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="32"/>
+        <v>65</v>
+      </c>
+      <c r="F12" s="38"/>
+      <c r="G12" s="41"/>
+      <c r="H12" s="38"/>
       <c r="I12" s="13"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:11" ht="27" x14ac:dyDescent="0.3">
-      <c r="A13" s="41"/>
+      <c r="A13" s="47"/>
       <c r="B13" s="16">
         <v>44673</v>
       </c>
-      <c r="C13" s="38"/>
+      <c r="C13" s="45"/>
       <c r="D13" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="F13" s="32"/>
-      <c r="G13" s="35"/>
-      <c r="H13" s="33"/>
+        <v>76</v>
+      </c>
+      <c r="F13" s="38"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="39"/>
       <c r="I13" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:11" ht="54" x14ac:dyDescent="0.3">
-      <c r="A14" s="41">
+      <c r="A14" s="47">
         <v>5</v>
       </c>
       <c r="B14" s="16">
         <v>44676</v>
       </c>
-      <c r="C14" s="38"/>
+      <c r="C14" s="45"/>
       <c r="D14" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E14" s="25" t="s">
-        <v>77</v>
-      </c>
-      <c r="F14" s="32"/>
-      <c r="G14" s="35"/>
-      <c r="H14" s="34" t="s">
-        <v>40</v>
+        <v>75</v>
+      </c>
+      <c r="F14" s="38"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="40" t="s">
+        <v>39</v>
       </c>
       <c r="I14" s="13"/>
       <c r="J14" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="54" x14ac:dyDescent="0.3">
-      <c r="A15" s="41"/>
+      <c r="A15" s="47"/>
       <c r="B15" s="16">
         <v>44678</v>
       </c>
-      <c r="C15" s="38"/>
+      <c r="C15" s="45"/>
       <c r="D15" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E15" s="25" t="s">
-        <v>79</v>
-      </c>
-      <c r="F15" s="32"/>
-      <c r="G15" s="35"/>
-      <c r="H15" s="35"/>
+        <v>77</v>
+      </c>
+      <c r="F15" s="38"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="41"/>
       <c r="I15" s="13"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:11" ht="54" x14ac:dyDescent="0.3">
-      <c r="A16" s="41"/>
+      <c r="A16" s="47"/>
       <c r="B16" s="16">
         <v>44680</v>
       </c>
-      <c r="C16" s="38"/>
+      <c r="C16" s="45"/>
       <c r="D16" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E16" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="F16" s="32"/>
-      <c r="G16" s="35"/>
-      <c r="H16" s="36"/>
+        <v>78</v>
+      </c>
+      <c r="F16" s="38"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="42"/>
       <c r="I16" s="13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:11" ht="54" x14ac:dyDescent="0.3">
-      <c r="A17" s="41">
+      <c r="A17" s="47">
         <v>6</v>
       </c>
       <c r="B17" s="17">
         <v>44683</v>
       </c>
-      <c r="C17" s="39"/>
+      <c r="C17" s="46"/>
       <c r="D17" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E17" s="44" t="s">
-        <v>81</v>
-      </c>
-      <c r="F17" s="32"/>
-      <c r="G17" s="36"/>
-      <c r="H17" s="31" t="s">
-        <v>24</v>
+        <v>26</v>
+      </c>
+      <c r="E17" s="35" t="s">
+        <v>79</v>
+      </c>
+      <c r="F17" s="38"/>
+      <c r="G17" s="42"/>
+      <c r="H17" s="37" t="s">
+        <v>23</v>
       </c>
       <c r="I17" s="13"/>
       <c r="J17" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K17" s="3"/>
     </row>
     <row r="18" spans="1:11" ht="26" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="41"/>
+      <c r="A18" s="47"/>
       <c r="B18" s="16">
         <v>44685</v>
       </c>
-      <c r="C18" s="37" t="s">
-        <v>29</v>
+      <c r="C18" s="44" t="s">
+        <v>28</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="F18" s="33"/>
-      <c r="G18" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="H18" s="32"/>
+        <v>80</v>
+      </c>
+      <c r="F18" s="39"/>
+      <c r="G18" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="H18" s="38"/>
       <c r="I18" s="13"/>
       <c r="J18" s="5"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="41"/>
+      <c r="A19" s="47"/>
       <c r="B19" s="16">
         <v>44687</v>
       </c>
-      <c r="C19" s="38"/>
+      <c r="C19" s="45"/>
       <c r="D19" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="F19" s="5"/>
-      <c r="G19" s="35"/>
-      <c r="H19" s="33"/>
+        <v>82</v>
+      </c>
+      <c r="F19" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" s="41"/>
+      <c r="H19" s="39"/>
       <c r="I19" s="13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="J19" s="5"/>
     </row>
     <row r="20" spans="1:11" ht="81" x14ac:dyDescent="0.3">
-      <c r="A20" s="41">
+      <c r="A20" s="47">
         <v>7</v>
       </c>
       <c r="B20" s="16">
         <v>44690</v>
       </c>
-      <c r="C20" s="38"/>
+      <c r="C20" s="45"/>
       <c r="D20" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E20" s="25" t="s">
-        <v>88</v>
-      </c>
-      <c r="F20" s="5"/>
-      <c r="G20" s="35"/>
-      <c r="H20" s="31" t="s">
-        <v>41</v>
+        <v>84</v>
+      </c>
+      <c r="F20" s="41"/>
+      <c r="G20" s="41"/>
+      <c r="H20" s="37" t="s">
+        <v>40</v>
       </c>
       <c r="I20" s="13"/>
       <c r="J20" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="K20" s="45" t="s">
-        <v>83</v>
+        <v>48</v>
+      </c>
+      <c r="K20" s="36" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" s="41"/>
+      <c r="A21" s="47"/>
       <c r="B21" s="18">
         <v>44692</v>
       </c>
-      <c r="C21" s="38"/>
+      <c r="C21" s="45"/>
       <c r="D21" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="F21" s="5"/>
-      <c r="G21" s="35"/>
-      <c r="H21" s="32"/>
+        <v>85</v>
+      </c>
+      <c r="F21" s="41"/>
+      <c r="G21" s="41"/>
+      <c r="H21" s="38"/>
       <c r="I21" s="13"/>
       <c r="J21" s="5"/>
     </row>
     <row r="22" spans="1:11" ht="26" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="41"/>
+      <c r="A22" s="47"/>
       <c r="B22" s="16">
         <v>44694</v>
       </c>
-      <c r="C22" s="38"/>
+      <c r="C22" s="45"/>
       <c r="D22" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F22" s="5"/>
-      <c r="G22" s="35"/>
-      <c r="H22" s="33"/>
+        <v>33</v>
+      </c>
+      <c r="F22" s="41"/>
+      <c r="G22" s="41"/>
+      <c r="H22" s="39"/>
       <c r="I22" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J22" s="5"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A23" s="41">
+      <c r="A23" s="47">
         <v>8</v>
       </c>
       <c r="B23" s="18">
         <v>44697</v>
       </c>
-      <c r="C23" s="38"/>
+      <c r="C23" s="45"/>
       <c r="D23" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="35"/>
-      <c r="H23" s="31" t="s">
-        <v>86</v>
+        <v>33</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F23" s="41"/>
+      <c r="G23" s="41"/>
+      <c r="H23" s="37" t="s">
+        <v>83</v>
       </c>
       <c r="I23" s="13"/>
       <c r="J23" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K23" s="7"/>
     </row>
     <row r="24" spans="1:11" ht="26" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="41"/>
+      <c r="A24" s="47"/>
       <c r="B24" s="19">
         <v>44699</v>
       </c>
-      <c r="C24" s="39"/>
+      <c r="C24" s="46"/>
       <c r="D24" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="G24" s="36"/>
-      <c r="H24" s="32"/>
+        <v>33</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="F24" s="42"/>
+      <c r="G24" s="42"/>
+      <c r="H24" s="38"/>
       <c r="I24" s="13"/>
       <c r="J24" s="5"/>
       <c r="K24" s="3"/>
     </row>
     <row r="25" spans="1:11" ht="54" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="41"/>
+      <c r="A25" s="47"/>
       <c r="B25" s="16">
         <v>44701</v>
       </c>
-      <c r="C25" s="32" t="s">
+      <c r="C25" s="38" t="s">
         <v>9</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="34" t="s">
-        <v>12</v>
-      </c>
-      <c r="H25" s="33"/>
+        <v>35</v>
+      </c>
+      <c r="E25" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="F25" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="G25" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="H25" s="39"/>
       <c r="I25" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J25" s="5"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A26" s="41">
+      <c r="A26" s="47">
         <v>9</v>
       </c>
       <c r="B26" s="16">
         <v>44704</v>
       </c>
-      <c r="C26" s="32"/>
+      <c r="C26" s="38"/>
       <c r="D26" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="35"/>
-      <c r="H26" s="31" t="s">
-        <v>87</v>
+        <v>36</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="F26" s="41"/>
+      <c r="G26" s="41"/>
+      <c r="H26" s="37" t="s">
+        <v>93</v>
       </c>
       <c r="I26" s="13"/>
       <c r="J26" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A27" s="41"/>
+      <c r="A27" s="47"/>
       <c r="B27" s="16">
         <v>44706</v>
       </c>
-      <c r="C27" s="32"/>
+      <c r="C27" s="38"/>
       <c r="D27" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="35"/>
-      <c r="H27" s="32"/>
+        <v>37</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F27" s="41"/>
+      <c r="G27" s="41"/>
+      <c r="H27" s="38"/>
       <c r="I27" s="13"/>
       <c r="J27" s="5"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A28" s="41"/>
+      <c r="A28" s="47"/>
       <c r="B28" s="19">
         <v>44708</v>
       </c>
-      <c r="C28" s="33"/>
+      <c r="C28" s="39"/>
       <c r="D28" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="36"/>
-      <c r="H28" s="33"/>
+        <v>37</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F28" s="42"/>
+      <c r="G28" s="42"/>
+      <c r="H28" s="39"/>
       <c r="I28" s="14" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J28" s="4"/>
       <c r="K28" s="2"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A29" s="41">
+      <c r="A29" s="47">
         <v>10</v>
       </c>
       <c r="B29" s="20">
@@ -1699,42 +1737,50 @@
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A30" s="41"/>
+      <c r="A30" s="47"/>
       <c r="B30" s="16">
         <v>44713</v>
       </c>
-      <c r="C30" s="32" t="s">
+      <c r="C30" s="38" t="s">
+        <v>91</v>
+      </c>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="F30" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
       <c r="G30" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="H30" s="31" t="s">
-        <v>57</v>
+        <v>10</v>
+      </c>
+      <c r="H30" s="37" t="s">
+        <v>90</v>
       </c>
       <c r="I30" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A31" s="41"/>
+      <c r="A31" s="47"/>
       <c r="B31" s="19">
         <v>44715</v>
       </c>
-      <c r="C31" s="33"/>
+      <c r="C31" s="39"/>
       <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
+      <c r="E31" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="F31" s="32" t="s">
+        <v>11</v>
+      </c>
       <c r="G31" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="H31" s="33"/>
+        <v>11</v>
+      </c>
+      <c r="H31" s="39"/>
       <c r="I31" s="14"/>
       <c r="J31" s="4"/>
       <c r="K31" s="2" t="s">
@@ -1752,7 +1798,7 @@
       <c r="G32" s="5"/>
       <c r="H32" s="5"/>
       <c r="I32" s="28" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="J32" s="5"/>
     </row>
@@ -1801,7 +1847,7 @@
       <c r="J36" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="31">
+  <mergeCells count="33">
     <mergeCell ref="A17:A19"/>
     <mergeCell ref="A20:A22"/>
     <mergeCell ref="A23:A25"/>
@@ -1823,6 +1869,8 @@
     <mergeCell ref="C9:C17"/>
     <mergeCell ref="F2:F9"/>
     <mergeCell ref="F10:F18"/>
+    <mergeCell ref="F19:F24"/>
+    <mergeCell ref="F25:F28"/>
     <mergeCell ref="H20:H22"/>
     <mergeCell ref="H23:H25"/>
     <mergeCell ref="H26:H28"/>

</xml_diff>